<commit_message>
masterfile updated questions WIP
</commit_message>
<xml_diff>
--- a/df_GRI_v2.xlsx
+++ b/df_GRI_v2.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Unistra\Unistra\Recherche\RAGbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DD0588-D562-47D6-B86E-313DD95C7BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4075D385-BAE5-420B-87D2-234C58C48D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="279">
   <si>
     <t>ID</t>
   </si>
@@ -857,6 +870,69 @@
   </si>
   <si>
     <t>['Co-participant', 'Components', 'Depictive', 'Instrument', 'Manner', 'Means', 'Place', 'Purpose', 'Role', 'Time']</t>
+  </si>
+  <si>
+    <t>E15</t>
+  </si>
+  <si>
+    <t>Multi Quantity</t>
+  </si>
+  <si>
+    <t>('sites' : int64, 'hectares' : float64)</t>
+  </si>
+  <si>
+    <t>('sites' : 13, 'hectares' : 23.4)</t>
+  </si>
+  <si>
+    <t>('sites' : NaN, 'hectares' : NaN)</t>
+  </si>
+  <si>
+    <t>E16</t>
+  </si>
+  <si>
+    <t>Single Quantity</t>
+  </si>
+  <si>
+    <t>('sites' : int64)</t>
+  </si>
+  <si>
+    <t>('sites' : 13)</t>
+  </si>
+  <si>
+    <t>('sites' : NaN)</t>
+  </si>
+  <si>
+    <t>E17</t>
+  </si>
+  <si>
+    <t>('hectares' : float64)</t>
+  </si>
+  <si>
+    <t>('hectares' : 23.4)</t>
+  </si>
+  <si>
+    <t>('hectares' : NaN)</t>
+  </si>
+  <si>
+    <t>E11</t>
+  </si>
+  <si>
+    <t>E12</t>
+  </si>
+  <si>
+    <t>E13</t>
+  </si>
+  <si>
+    <t>E14</t>
+  </si>
+  <si>
+    <t>E16. Veuillez indiquer le nombre des sites possédés, loués ou gérés par l'entreprise dans ou à proximité d'aires protégées et / ou de zones clés pour la biodiversité (KBA).</t>
+  </si>
+  <si>
+    <t>E17. Veuillez indiquer la superficie (en hectares) des sites possédés, loués ou gérés par l'entreprise dans ou à proximité d'aires protégées et / ou de zones clés pour la biodiversité (KBA).</t>
+  </si>
+  <si>
+    <t>E15. Veuillez indiquer le nombre et la superficie (en hectares) des sites possédés, loués ou gérés par l'entreprise dans ou à proximité d'aires protégées et / ou de zones clés pour la biodiversité (KBA).</t>
   </si>
 </sst>
 </file>
@@ -1222,15 +1298,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="138.5546875" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
@@ -2214,6 +2290,86 @@
         <v>252</v>
       </c>
     </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" t="s">
+        <v>278</v>
+      </c>
+      <c r="C22" t="s">
+        <v>259</v>
+      </c>
+      <c r="J22" t="s">
+        <v>260</v>
+      </c>
+      <c r="K22" t="s">
+        <v>261</v>
+      </c>
+      <c r="M22" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>263</v>
+      </c>
+      <c r="B23" t="s">
+        <v>276</v>
+      </c>
+      <c r="C23" t="s">
+        <v>264</v>
+      </c>
+      <c r="J23" t="s">
+        <v>265</v>
+      </c>
+      <c r="K23" t="s">
+        <v>266</v>
+      </c>
+      <c r="M23" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>268</v>
+      </c>
+      <c r="B24" t="s">
+        <v>277</v>
+      </c>
+      <c r="C24" t="s">
+        <v>264</v>
+      </c>
+      <c r="J24" t="s">
+        <v>269</v>
+      </c>
+      <c r="K24" t="s">
+        <v>270</v>
+      </c>
+      <c r="M24" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>